<commit_message>
Initial draft of heuristics (last modified September 23rd, 2019)
</commit_message>
<xml_diff>
--- a/resources/heuristics-db-connection.xlsx
+++ b/resources/heuristics-db-connection.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vanessa/workspace/db-mining/docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vanessa/workspace/db-mining/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73AA93FE-F2C1-8D47-B59E-B6CC1A794624}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C40A6C9B-7839-A742-9DE7-06E35DFA78E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5480" yWindow="2300" windowWidth="27840" windowHeight="17060" activeTab="1" xr2:uid="{A3FFBE04-F7A1-054D-B76D-7AC781316E0A}"/>
+    <workbookView xWindow="5480" yWindow="2300" windowWidth="27840" windowHeight="17060" activeTab="2" xr2:uid="{A3FFBE04-F7A1-054D-B76D-7AC781316E0A}"/>
   </bookViews>
   <sheets>
     <sheet name="Heuristics for Specific DBs" sheetId="1" r:id="rId1"/>
     <sheet name="Generic Heuristics" sheetId="2" r:id="rId2"/>
+    <sheet name="Projects" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="55">
   <si>
     <t>MySQL</t>
   </si>
@@ -148,13 +149,64 @@
   </si>
   <si>
     <t>(for Ruby)</t>
+  </si>
+  <si>
+    <t>owner</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>Database</t>
+  </si>
+  <si>
+    <t>Activiti</t>
+  </si>
+  <si>
+    <t>OBS</t>
+  </si>
+  <si>
+    <t>Arquivo pom.xml tem referência apenas para H2</t>
+  </si>
+  <si>
+    <t>Evidência</t>
+  </si>
+  <si>
+    <t>activiti-engine/src/main/java/org/activiti/engine/impl/AbstractQuery.java</t>
+  </si>
+  <si>
+    <t>H2; HSQL; MySQL; PostgreSQL; DB2; SQL Server; Oracle</t>
+  </si>
+  <si>
+    <t>activiti-engine/src/main/java/org/activiti/engine/impl/cfg/ProcessEngineConfigurationImpl.java</t>
+  </si>
+  <si>
+    <t>Tipo Heurística</t>
+  </si>
+  <si>
+    <t>Impl</t>
+  </si>
+  <si>
+    <t>SQL para criar o BD</t>
+  </si>
+  <si>
+    <t>activiti-engine/src/main/resources/org/activiti/db/create</t>
+  </si>
+  <si>
+    <t>Framework MOR MyBatis (https://blog.mybatis.org/p/about.html)</t>
+  </si>
+  <si>
+    <t>activiti-engine/src/main/resources/org/activiti/db/mapping/entity/Attachment.xml</t>
+  </si>
+  <si>
+    <t>pom.xml</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -177,6 +229,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Menlo"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -212,7 +270,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -222,9 +280,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -241,7 +302,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -724,8 +785,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ED21265-E6AA-1146-B786-26EE816D5941}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -763,4 +824,94 @@
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55BFB640-B9B6-7041-9717-AC28637DC937}">
+  <dimension ref="A1:E8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="88.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="41.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="E3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D4" s="8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C5" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C6" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C7" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D8" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>